<commit_message>
Logic filtererd as per transpose
</commit_message>
<xml_diff>
--- a/validatedata.xlsx
+++ b/validatedata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravin\Documents\DATA ANALYSIS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F273EA-29FE-45AA-8185-17B40AB3661E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D6EEB5-72AD-4A6D-8658-960993DA30E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{64BEA55E-C568-4FB0-9BD3-2F73692D65BF}"/>
   </bookViews>
@@ -21,15 +21,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -373,7 +364,7 @@
     <t>Domain</t>
   </si>
   <si>
-    <t>Region</t>
+    <t>UserGroup</t>
   </si>
 </sst>
 </file>
@@ -424,11 +415,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -774,7 +762,7 @@
   <dimension ref="A1:B215"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,926 +780,906 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3" t="s">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3" t="s">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="3" t="s">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3" t="s">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3" t="s">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3" t="s">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3" t="s">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3" t="s">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3" t="s">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3" t="s">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3" t="s">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3" t="s">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3" t="s">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="4" t="s">
+      <c r="A49" s="2"/>
+      <c r="B49" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-      <c r="B51" s="4" t="s">
+      <c r="A51" s="2"/>
+      <c r="B51" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="4" t="s">
+      <c r="A53" s="2"/>
+      <c r="B53" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="B55" s="4" t="s">
+      <c r="A55" s="2"/>
+      <c r="B55" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="B57" s="4" t="s">
+      <c r="A57" s="2"/>
+      <c r="B57" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
-      <c r="B59" s="4" t="s">
+      <c r="A59" s="2"/>
+      <c r="B59" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-      <c r="B61" s="4" t="s">
+      <c r="A61" s="2"/>
+      <c r="B61" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="3"/>
-      <c r="B63" s="4" t="s">
+      <c r="A63" s="2"/>
+      <c r="B63" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="3"/>
-      <c r="B65" s="4" t="s">
+      <c r="A65" s="2"/>
+      <c r="B65" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3" t="s">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="3"/>
-      <c r="B69" s="3" t="s">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3" t="s">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3" t="s">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3" t="s">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3" t="s">
+      <c r="A77" s="2"/>
+      <c r="B77" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="2" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3" t="s">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="2" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="3"/>
-      <c r="B81" s="3" t="s">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="3"/>
-      <c r="B83" s="3" t="s">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="3"/>
-      <c r="B85" s="3" t="s">
+      <c r="A85" s="2"/>
+      <c r="B85" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="3"/>
-      <c r="B87" s="3" t="s">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="3"/>
-      <c r="B89" s="3" t="s">
+      <c r="A89" s="2"/>
+      <c r="B89" s="2" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="3"/>
-      <c r="B91" s="3" t="s">
+      <c r="A91" s="2"/>
+      <c r="B91" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="3" t="s">
+      <c r="B92" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="3"/>
+      <c r="A93" s="2"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="4"/>
+      <c r="B94" s="3"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="3"/>
+      <c r="A95" s="2"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="4"/>
+      <c r="B96" s="3"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="3"/>
+      <c r="A97" s="2"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="4"/>
+      <c r="B98" s="3"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="3"/>
+      <c r="A99" s="2"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="4"/>
+      <c r="B100" s="3"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="3"/>
+      <c r="A101" s="2"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="4"/>
+      <c r="B102" s="3"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="3"/>
+      <c r="A103" s="2"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="4"/>
+      <c r="B104" s="3"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="3"/>
+      <c r="A105" s="2"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="4"/>
+      <c r="B106" s="3"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="3"/>
+      <c r="A107" s="2"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="4"/>
+      <c r="B108" s="3"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="3"/>
+      <c r="A109" s="2"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="4"/>
+      <c r="B110" s="3"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="3"/>
+      <c r="A111" s="2"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="4"/>
+      <c r="B112" s="3"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="3"/>
+      <c r="A113" s="2"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="4"/>
+      <c r="B114" s="3"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="3"/>
+      <c r="A115" s="2"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="4"/>
+      <c r="B116" s="3"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="3"/>
+      <c r="A117" s="2"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="4"/>
+      <c r="B118" s="3"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="3"/>
+      <c r="A119" s="2"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="4"/>
+      <c r="B120" s="3"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="3"/>
+      <c r="A121" s="2"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B122" s="4"/>
+      <c r="B122" s="3"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="4"/>
+      <c r="A123" s="3"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="4"/>
+      <c r="B124" s="3"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="4"/>
+      <c r="A125" s="3"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B126" s="4"/>
+      <c r="B126" s="3"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="4"/>
+      <c r="A127" s="3"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B128" s="4"/>
+      <c r="B128" s="3"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="4"/>
+      <c r="A129" s="3"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B130" s="3"/>
+      <c r="B130" s="2"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="4"/>
+      <c r="A131" s="3"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B132" s="3"/>
+      <c r="B132" s="2"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="4"/>
+      <c r="A133" s="3"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B134" s="3"/>
+      <c r="B134" s="2"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="4"/>
+      <c r="A135" s="3"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="3"/>
+      <c r="B136" s="2"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="4"/>
+      <c r="A137" s="3"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="3"/>
+      <c r="B138" s="2"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="4"/>
+      <c r="A139" s="3"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B140" s="3"/>
+      <c r="B140" s="2"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="4"/>
+      <c r="A141" s="3"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B142" s="3"/>
+      <c r="B142" s="2"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="4"/>
+      <c r="A143" s="3"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B144" s="3"/>
+      <c r="B144" s="2"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="4"/>
+      <c r="A145" s="3"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B146" s="3"/>
+      <c r="B146" s="2"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="4"/>
+      <c r="A147" s="3"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B148" s="3"/>
+      <c r="B148" s="2"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="4"/>
+      <c r="A149" s="3"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B150" s="3"/>
+      <c r="B150" s="2"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="4"/>
+      <c r="A151" s="3"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B152" s="3"/>
+      <c r="B152" s="2"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="4"/>
+      <c r="A153" s="3"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B154" s="3"/>
+      <c r="B154" s="2"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="4"/>
+      <c r="A155" s="3"/>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B156" s="3"/>
+      <c r="B156" s="2"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="4"/>
+      <c r="A157" s="3"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B158" s="3"/>
+      <c r="B158" s="2"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="3"/>
+      <c r="A159" s="2"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B160" s="3"/>
+      <c r="B160" s="2"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="3"/>
+      <c r="A161" s="2"/>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B162" s="3"/>
+      <c r="B162" s="2"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="3"/>
+      <c r="A163" s="2"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B164" s="3"/>
+      <c r="B164" s="2"/>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="3"/>
+      <c r="A165" s="2"/>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B166" s="3"/>
+      <c r="B166" s="2"/>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="3"/>
+      <c r="A167" s="2"/>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B168" s="3"/>
+      <c r="B168" s="2"/>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="3"/>
+      <c r="A169" s="2"/>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B170" s="3"/>
+      <c r="B170" s="2"/>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" s="3"/>
+      <c r="A171" s="2"/>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B172" s="3"/>
+      <c r="B172" s="2"/>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" s="3"/>
+      <c r="A173" s="2"/>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B174" s="3"/>
+      <c r="B174" s="2"/>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" s="3"/>
+      <c r="A175" s="2"/>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B176" s="3"/>
+      <c r="B176" s="2"/>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" s="3"/>
+      <c r="A177" s="2"/>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B178" s="3"/>
+      <c r="B178" s="2"/>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" s="3"/>
+      <c r="A179" s="2"/>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B180" s="3"/>
+      <c r="B180" s="2"/>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" s="3"/>
+      <c r="A181" s="2"/>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B182" s="3"/>
+      <c r="B182" s="2"/>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" s="3"/>
+      <c r="A183" s="2"/>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" s="3"/>
+      <c r="A185" s="2"/>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B186" s="3"/>
+      <c r="B186" s="2"/>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" s="3"/>
-      <c r="B187" s="3"/>
+      <c r="A187" s="2"/>
+      <c r="B187" s="2"/>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B188" s="2"/>
+      <c r="B188" s="1"/>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A189" s="3"/>
+      <c r="A189" s="2"/>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A191" s="3"/>
+      <c r="A191" s="2"/>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="3"/>
+      <c r="A193" s="2"/>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="3"/>
+      <c r="A195" s="2"/>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="3"/>
+      <c r="A197" s="2"/>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="3"/>
+      <c r="A199" s="2"/>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A201" s="3"/>
+      <c r="A201" s="2"/>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="3"/>
+      <c r="A203" s="2"/>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" s="3"/>
+      <c r="A205" s="2"/>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A207" s="3"/>
+      <c r="A207" s="2"/>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="3"/>
+      <c r="A209" s="2"/>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" s="3"/>
+      <c r="A211" s="2"/>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="3"/>
+      <c r="A213" s="2"/>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" s="3"/>
+      <c r="A214" s="2"/>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A215" s="2"/>
+      <c r="A215" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" tooltip="http://www.dell.il/" display="http://www.dell.il/" xr:uid="{D8CE1A5A-8A97-48D1-9867-AA2308D8DD91}"/>
-    <hyperlink ref="A3" r:id="rId2" tooltip="http://www.dell.com.az/" display="http://www.dell.com.az/" xr:uid="{E7D46DBB-124C-4D83-A184-63F4F61832C0}"/>
-    <hyperlink ref="A4" r:id="rId3" tooltip="http://www.dell.com.sa/" display="http://www.dell.com.sa/" xr:uid="{06BBAE4C-2DEB-4F9E-BC47-5B887B62CE5F}"/>
-    <hyperlink ref="A5" r:id="rId4" tooltip="http://www.dell.com.cl/" display="http://www.dell.com.cl/" xr:uid="{0630F292-DA03-4BC7-9674-7086762EC78C}"/>
-    <hyperlink ref="A6" r:id="rId5" tooltip="http://www.dell.com.cr/" display="http://www.dell.com.cr/" xr:uid="{D010111D-7501-4B65-B392-7F594A34E998}"/>
-    <hyperlink ref="A7" r:id="rId6" tooltip="http://www.dell.com.an/" display="http://www.dell.com.an/" xr:uid="{35B6C21F-853A-4EC9-90B2-88E110BAE87A}"/>
-    <hyperlink ref="A8" r:id="rId7" tooltip="http://www.dell.com.aw/" display="http://www.dell.com.aw/" xr:uid="{1A1D8365-17D3-4553-B67F-C05F2657EC89}"/>
-    <hyperlink ref="A9" r:id="rId8" tooltip="http://www.dell.co.zw/" display="http://www.dell.co.zw/" xr:uid="{93270130-459F-4164-9D8A-0525AA1956FB}"/>
-    <hyperlink ref="A10" r:id="rId9" tooltip="http://www.dell.md/" display="http://www.dell.md/" xr:uid="{BAD5F6DC-3D77-4D92-BA6E-2BA736D9F779}"/>
-    <hyperlink ref="A11" r:id="rId10" tooltip="http://www.dell.com.dm/" display="http://www.dell.com.dm/" xr:uid="{EA3710DA-383E-46AC-91CA-ADAA8F5BAE0C}"/>
-    <hyperlink ref="A12" r:id="rId11" tooltip="http://www.dell.com.ae/" display="http://www.dell.com.ae/" xr:uid="{1DA377DE-D1D5-48E6-A062-75EA53C373DA}"/>
-    <hyperlink ref="A13" r:id="rId12" tooltip="http://www.dell.com.bm/" display="http://www.dell.com.bm/" xr:uid="{4E76344F-4E35-4252-832B-2104F598D25A}"/>
-    <hyperlink ref="A14" r:id="rId13" tooltip="http://www.dellnet.ie/" display="http://www.dellnet.ie/" xr:uid="{2F5F20A8-A0C5-49E0-980C-DC156B4BB865}"/>
-    <hyperlink ref="A15" r:id="rId14" tooltip="http://www.dellnet.ch/" display="http://www.dellnet.ch/" xr:uid="{A91EA809-0D16-4247-824E-3AF849026EF1}"/>
-    <hyperlink ref="A16" r:id="rId15" tooltip="http://www.dellcomputers.sk/" display="http://www.dellcomputers.sk/" xr:uid="{C45F2EEB-E2CA-4CB7-9EF2-3D2FC8F87372}"/>
-    <hyperlink ref="A17" r:id="rId16" tooltip="http://www.dellservicesevents.com/" display="http://www.dellservicesevents.com/" xr:uid="{6704EFBF-82AA-4E4D-B119-49C8071C8D54}"/>
-    <hyperlink ref="A18" r:id="rId17" tooltip="http://www.dell.no/" display="http://www.dell.no/" xr:uid="{22B36163-05DF-4F76-9E9F-A86ECB055E35}"/>
-    <hyperlink ref="A19" r:id="rId18" tooltip="http://www.dell.cd/" display="http://www.dell.cd/" xr:uid="{44473C5E-77D9-41D4-AD1D-47FC2CA9BDCD}"/>
-    <hyperlink ref="A20" r:id="rId19" tooltip="http://www.dell.cz/" display="http://www.dell.cz/" xr:uid="{B55E2DC8-DD62-4B66-AE57-AC080CD3B1FE}"/>
-    <hyperlink ref="A21" r:id="rId20" tooltip="http://www.dell.ae/" display="http://www.dell.ae/" xr:uid="{F8D227DB-FAFF-4357-B701-8BEDE4627389}"/>
-    <hyperlink ref="B48" r:id="rId21" tooltip="https://www.alienware.com.au/" display="https://www.alienware.com.au/" xr:uid="{B8BFE7CA-53E4-44E1-B4BF-5730192B7E66}"/>
-    <hyperlink ref="B49" r:id="rId22" tooltip="https://www.ap.dell.com/" display="https://www.ap.dell.com/" xr:uid="{5D6A4DE5-37C5-485F-A4BB-E90497C28D54}"/>
-    <hyperlink ref="B50" r:id="rId23" tooltip="https://www.dell.ca/" display="https://www.dell.ca/" xr:uid="{404F3D28-70AE-43C5-A62E-7F3EB195EC30}"/>
-    <hyperlink ref="B51" r:id="rId24" tooltip="https://www.dell.co.in/" display="https://www.dell.co.in/" xr:uid="{4341E0D6-D1DA-4465-923B-268F5579A311}"/>
-    <hyperlink ref="B52" r:id="rId25" tooltip="https://www.dell.co.kr/" display="https://www.dell.co.kr/" xr:uid="{0497E26E-0E4C-4400-9BDC-67392D923B76}"/>
-    <hyperlink ref="B53" r:id="rId26" tooltip="https://www.dell.co.nz/" display="https://www.dell.co.nz/" xr:uid="{031A38D2-2A32-4BF7-83E1-2FA9D6D0FA95}"/>
-    <hyperlink ref="B54" r:id="rId27" tooltip="https://www.dell.co.th/" display="https://www.dell.co.th/" xr:uid="{7A49DDA6-FD79-4E52-9327-F2E7155EC7DE}"/>
-    <hyperlink ref="B55" r:id="rId28" tooltip="https://www.dell.com/" display="https://www.dell.com/" xr:uid="{8D1CE617-EF97-4FAC-BDDE-935861B46234}"/>
-    <hyperlink ref="B56" r:id="rId29" tooltip="https://www.dell.com.au/" display="https://www.dell.com.au/" xr:uid="{1404FDF8-E5A5-40F1-ABBB-640A510B62C3}"/>
-    <hyperlink ref="B57" r:id="rId30" tooltip="https://www.dell.com.cn/" display="https://www.dell.com.cn/" xr:uid="{345BBF7C-591D-48FB-BB03-BB1D4C52A0B4}"/>
-    <hyperlink ref="B58" r:id="rId31" tooltip="https://www.dell.com.hk/" display="https://www.dell.com.hk/" xr:uid="{3580C334-BB3B-41AF-80C6-D268E9238493}"/>
-    <hyperlink ref="B59" r:id="rId32" tooltip="https://www.dell.com.my/" display="https://www.dell.com.my/" xr:uid="{664715FD-2C05-4812-BCC7-13147EC8E442}"/>
-    <hyperlink ref="B60" r:id="rId33" tooltip="https://www.dell.com.sg/" display="https://www.dell.com.sg/" xr:uid="{3B7F3CDA-CA74-40D6-95C5-71BC96FCA622}"/>
-    <hyperlink ref="B61" r:id="rId34" tooltip="https://www.dell.com.tw/" display="https://www.dell.com.tw/" xr:uid="{B62F55C3-E9FA-4417-B3A4-15615DA0721D}"/>
-    <hyperlink ref="B62" r:id="rId35" tooltip="https://www.dell.id/" display="https://www.dell.id/" xr:uid="{F2EC3E3D-B1A9-43C0-BFBD-136DC8103549}"/>
-    <hyperlink ref="B63" r:id="rId36" tooltip="https://www.dell.ph/" display="https://www.dell.ph/" xr:uid="{0348C50C-B548-46EF-9AF1-165C6A4C5716}"/>
-    <hyperlink ref="B64" r:id="rId37" tooltip="https://www.dell.vn/" display="https://www.dell.vn/" xr:uid="{B9E753F7-36FD-4820-8703-D61875F61A72}"/>
-    <hyperlink ref="B65" r:id="rId38" tooltip="https://www.jp.dell.com/" display="https://www.jp.dell.com/" xr:uid="{E4A09ACE-0530-4BB9-B7B1-3B479D041B42}"/>
+    <hyperlink ref="B48" r:id="rId1" tooltip="https://www.alienware.com.au/" display="https://www.alienware.com.au/" xr:uid="{B8BFE7CA-53E4-44E1-B4BF-5730192B7E66}"/>
+    <hyperlink ref="B49" r:id="rId2" tooltip="https://www.ap.dell.com/" display="https://www.ap.dell.com/" xr:uid="{5D6A4DE5-37C5-485F-A4BB-E90497C28D54}"/>
+    <hyperlink ref="B50" r:id="rId3" tooltip="https://www.dell.ca/" display="https://www.dell.ca/" xr:uid="{404F3D28-70AE-43C5-A62E-7F3EB195EC30}"/>
+    <hyperlink ref="B51" r:id="rId4" tooltip="https://www.dell.co.in/" display="https://www.dell.co.in/" xr:uid="{4341E0D6-D1DA-4465-923B-268F5579A311}"/>
+    <hyperlink ref="B52" r:id="rId5" tooltip="https://www.dell.co.kr/" display="https://www.dell.co.kr/" xr:uid="{0497E26E-0E4C-4400-9BDC-67392D923B76}"/>
+    <hyperlink ref="B53" r:id="rId6" tooltip="https://www.dell.co.nz/" display="https://www.dell.co.nz/" xr:uid="{031A38D2-2A32-4BF7-83E1-2FA9D6D0FA95}"/>
+    <hyperlink ref="B54" r:id="rId7" tooltip="https://www.dell.co.th/" display="https://www.dell.co.th/" xr:uid="{7A49DDA6-FD79-4E52-9327-F2E7155EC7DE}"/>
+    <hyperlink ref="B55" r:id="rId8" tooltip="https://www.dell.com/" display="https://www.dell.com/" xr:uid="{8D1CE617-EF97-4FAC-BDDE-935861B46234}"/>
+    <hyperlink ref="B56" r:id="rId9" tooltip="https://www.dell.com.au/" display="https://www.dell.com.au/" xr:uid="{1404FDF8-E5A5-40F1-ABBB-640A510B62C3}"/>
+    <hyperlink ref="B57" r:id="rId10" tooltip="https://www.dell.com.cn/" display="https://www.dell.com.cn/" xr:uid="{345BBF7C-591D-48FB-BB03-BB1D4C52A0B4}"/>
+    <hyperlink ref="B58" r:id="rId11" tooltip="https://www.dell.com.hk/" display="https://www.dell.com.hk/" xr:uid="{3580C334-BB3B-41AF-80C6-D268E9238493}"/>
+    <hyperlink ref="B59" r:id="rId12" tooltip="https://www.dell.com.my/" display="https://www.dell.com.my/" xr:uid="{664715FD-2C05-4812-BCC7-13147EC8E442}"/>
+    <hyperlink ref="B60" r:id="rId13" tooltip="https://www.dell.com.sg/" display="https://www.dell.com.sg/" xr:uid="{3B7F3CDA-CA74-40D6-95C5-71BC96FCA622}"/>
+    <hyperlink ref="B61" r:id="rId14" tooltip="https://www.dell.com.tw/" display="https://www.dell.com.tw/" xr:uid="{B62F55C3-E9FA-4417-B3A4-15615DA0721D}"/>
+    <hyperlink ref="B62" r:id="rId15" tooltip="https://www.dell.id/" display="https://www.dell.id/" xr:uid="{F2EC3E3D-B1A9-43C0-BFBD-136DC8103549}"/>
+    <hyperlink ref="B63" r:id="rId16" tooltip="https://www.dell.ph/" display="https://www.dell.ph/" xr:uid="{0348C50C-B548-46EF-9AF1-165C6A4C5716}"/>
+    <hyperlink ref="B64" r:id="rId17" tooltip="https://www.dell.vn/" display="https://www.dell.vn/" xr:uid="{B9E753F7-36FD-4820-8703-D61875F61A72}"/>
+    <hyperlink ref="B65" r:id="rId18" tooltip="https://www.jp.dell.com/" display="https://www.jp.dell.com/" xr:uid="{E4A09ACE-0530-4BB9-B7B1-3B479D041B42}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1728,457 +1696,457 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="2" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="2" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="2" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="2" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>